<commit_message>
Validate batch ingest packages before proceeding with ingest
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="5680" yWindow="2440" windowWidth="30280" windowHeight="17840" tabRatio="500"/>
@@ -27,9 +27,6 @@
     <t>Creator</t>
   </si>
   <si>
-    <t>Date Created</t>
-  </si>
-  <si>
     <t>Adam Hallett</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>California</t>
+  </si>
+  <si>
+    <t>Date Issued</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -451,13 +451,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -469,23 +469,23 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>2012</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add specs for new batch features
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="2440" windowWidth="30280" windowHeight="17840" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="30280" windowHeight="17840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Main Title</t>
   </si>
@@ -27,29 +27,53 @@
     <t>Creator</t>
   </si>
   <si>
-    <t>Adam Hallett</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>adam.hallett@northwestern.edu</t>
-  </si>
-  <si>
     <t>assets/sheephead_mountain.mov</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
     <t>Date Issued</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>00:00:00.500</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>Frances Dickens</t>
+  </si>
+  <si>
+    <t>frances.dickens@reichel.com</t>
+  </si>
+  <si>
+    <t>Carroll, Nora</t>
+  </si>
+  <si>
+    <t>Ut minus ut accusantium odio autem odit.</t>
+  </si>
+  <si>
+    <t>Quis quo</t>
+  </si>
+  <si>
+    <t>Dolorum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,14 +93,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,18 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,32 +450,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.1640625" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,33 +486,48 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>2012</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:7">
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Add "skip transcoding" support to batch ingest
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="440" windowWidth="30280" windowHeight="17840" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Main Title</t>
   </si>
@@ -67,13 +67,22 @@
   </si>
   <si>
     <t>Dolorum</t>
+  </si>
+  <si>
+    <t>Unde aliquid</t>
+  </si>
+  <si>
+    <t>Skip Transcoding</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,6 +102,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,8 +136,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -120,7 +153,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -464,9 +505,12 @@
     <col min="5" max="5" width="42.1640625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -478,7 +522,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +544,20 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -523,9 +579,18 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="F4" s="1"/>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix bug/VOV-2840: collection column mishandled
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -206,13 +206,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add test for identifier/type ingest
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -53,6 +53,12 @@
     <t>Absolute Location</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Identifier Type</t>
+  </si>
+  <si>
     <t>Dolorum</t>
   </si>
   <si>
@@ -87,6 +93,15 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>BIB</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>OCLC</t>
   </si>
   <si>
     <t>Laborum</t>
@@ -209,10 +224,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -294,76 +309,100 @@
       <c r="P2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="Q2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add related item and terms of use
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -95,13 +95,7 @@
     <t>no</t>
   </si>
   <si>
-    <t>BIB</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>OCLC</t>
+    <t>Catalog Key</t>
   </si>
   <si>
     <t>Laborum</t>
@@ -224,10 +218,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -315,12 +309,6 @@
       <c r="R2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -375,19 +363,13 @@
       <c r="R3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
@@ -396,7 +378,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Add new fields to batch tests
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -59,6 +59,21 @@
     <t>Identifier Type</t>
   </si>
   <si>
+    <t>Related Item</t>
+  </si>
+  <si>
+    <t>Related Item Label</t>
+  </si>
+  <si>
+    <t>Terms of Use</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Original Physical Description</t>
+  </si>
+  <si>
     <t>Dolorum</t>
   </si>
   <si>
@@ -95,7 +110,22 @@
     <t>no</t>
   </si>
   <si>
-    <t>Catalog Key</t>
+    <t>local</t>
+  </si>
+  <si>
+    <t>http://www.example.com/text.pdf</t>
+  </si>
+  <si>
+    <t>Example Item PDF</t>
+  </si>
+  <si>
+    <t>Terms of Use Language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>16mm Reel</t>
   </si>
   <si>
     <t>Laborum</t>
@@ -218,10 +248,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -242,7 +272,14 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.3333333333333"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.9962962962963"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.537037037037"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.6666666666667"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.9962962962963"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="23.937037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -309,82 +346,112 @@
       <c r="R2" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="S2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>123</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix batch ingest of single-value fields
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -77,6 +77,12 @@
     <t>Absolute Location</t>
   </si>
   <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Statement Of Responsibility</t>
+  </si>
+  <si>
     <t>Dolorum</t>
   </si>
   <si>
@@ -129,6 +135,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Test abstract</t>
+  </si>
+  <si>
+    <t>Test Statement of Responsibility</t>
   </si>
   <si>
     <t>Laborum</t>
@@ -260,13 +272,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y4" activeCellId="0" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -358,108 +370,123 @@
       <c r="X2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="Y2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow batch and api to set date_ingested on masterfiles
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>Date Ingested</t>
   </si>
   <si>
     <t>Skip Transcoding</t>
@@ -168,8 +171,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -244,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,6 +258,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,17 +287,19 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y4" activeCellId="0" sqref="Y4"/>
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.84074074074074"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="22" min="6" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.5037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.84074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -347,85 +361,91 @@
         <v>17</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>42307</v>
+      </c>
+      <c r="R3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="T3" s="0" t="s">
         <v>35</v>
@@ -436,62 +456,71 @@
       <c r="V3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="4" t="n">
+        <v>42308</v>
+      </c>
+      <c r="X3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="Y3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Z3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
         <v>41</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="4" t="n">
+        <v>42302</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
+    <hyperlink ref="V3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fix tests and batch for date_digitized
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -71,7 +71,7 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Date Ingested</t>
+    <t>Date Digitized</t>
   </si>
   <si>
     <t>Skip Transcoding</t>
@@ -289,7 +289,7 @@
   </sheetPr>
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add special batch handling for other_identifier
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -41,6 +41,12 @@
     <t>Bibliographic ID Label</t>
   </si>
   <si>
+    <t>Other Identifier</t>
+  </si>
+  <si>
+    <t>Other Identifier Type</t>
+  </si>
+  <si>
     <t>Related Item URL</t>
   </si>
   <si>
@@ -92,6 +98,12 @@
     <t>Carroll, Nora</t>
   </si>
   <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
     <t>http://www.example.com/text.pdf</t>
   </si>
   <si>
@@ -162,9 +174,6 @@
   </si>
   <si>
     <t>7763100</t>
-  </si>
-  <si>
-    <t>local</t>
   </si>
 </sst>
 </file>
@@ -287,19 +296,20 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.84074074074074"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9925925925926"/>
-    <col collapsed="false" hidden="false" max="22" min="6" style="0" width="8.84074074074074"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.5037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3703703703704"/>
+    <col collapsed="false" hidden="false" max="24" min="7" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.5037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.84074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -309,7 +319,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -351,10 +361,10 @@
       <c r="M2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="0" t="s">
         <v>16</v>
       </c>
       <c r="P2" s="2" t="s">
@@ -364,163 +374,175 @@
         <v>18</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AB2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="0" t="s">
-        <v>22</v>
+      <c r="AC2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="N3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="P3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3" t="n">
         <v>42307</v>
       </c>
-      <c r="R3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="T3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="U3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="V3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="4" t="n">
         <v>42308</v>
       </c>
-      <c r="X3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="Z3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="4" t="n">
+        <v>42302</v>
+      </c>
+      <c r="AC4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="W4" s="4" t="n">
-        <v>42302</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
+    <hyperlink ref="X3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add special batch handling for other_identifier (#2148)
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Frances Dickens</t>
   </si>
@@ -41,6 +41,12 @@
     <t>Bibliographic ID Label</t>
   </si>
   <si>
+    <t>Other Identifier</t>
+  </si>
+  <si>
+    <t>Other Identifier Type</t>
+  </si>
+  <si>
     <t>Related Item URL</t>
   </si>
   <si>
@@ -92,6 +98,12 @@
     <t>Carroll, Nora</t>
   </si>
   <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
     <t>http://www.example.com/text.pdf</t>
   </si>
   <si>
@@ -162,9 +174,6 @@
   </si>
   <si>
     <t>7763100</t>
-  </si>
-  <si>
-    <t>local</t>
   </si>
 </sst>
 </file>
@@ -287,19 +296,20 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.84074074074074"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9925925925926"/>
-    <col collapsed="false" hidden="false" max="22" min="6" style="0" width="8.84074074074074"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.5037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3703703703704"/>
+    <col collapsed="false" hidden="false" max="24" min="7" style="0" width="8.84074074074074"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.5037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.84074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -309,7 +319,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -351,10 +361,10 @@
       <c r="M2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="0" t="s">
         <v>16</v>
       </c>
       <c r="P2" s="2" t="s">
@@ -364,163 +374,175 @@
         <v>18</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AB2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="0" t="s">
-        <v>22</v>
+      <c r="AC2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="N3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="P3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3" t="n">
         <v>42307</v>
       </c>
-      <c r="R3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="T3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="U3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="V3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="4" t="n">
         <v>42308</v>
       </c>
-      <c r="X3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="Z3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="4" t="n">
+        <v>42302</v>
+      </c>
+      <c r="AC4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="W4" s="4" t="n">
-        <v>42302</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
+    <hyperlink ref="X3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Restrict caption files to individual masterfiles
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -73,6 +73,18 @@
     <t xml:space="preserve">Note Type</t>
   </si>
   <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Digitized</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caption File</t>
   </si>
   <si>
@@ -82,18 +94,6 @@
     <t xml:space="preserve">Caption Language</t>
   </si>
   <si>
-    <t xml:space="preserve">File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Digitized</t>
-  </si>
-  <si>
     <t xml:space="preserve">Skip Transcoding</t>
   </si>
   <si>
@@ -139,19 +139,19 @@
     <t xml:space="preserve">general</t>
   </si>
   <si>
+    <t xml:space="preserve">assets/sheephead_mountain.mov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:00:00.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quis quo</t>
+  </si>
+  <si>
     <t xml:space="preserve">assets/sheephead_mountain.mov.vtt</t>
   </si>
   <si>
     <t xml:space="preserve">Sheephead Captions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assets/sheephead_mountain.mov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00:00:00.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quis quo</t>
   </si>
   <si>
     <t xml:space="preserve">Unde aliquid</t>
@@ -318,11 +318,11 @@
   </sheetPr>
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.37"/>
@@ -336,7 +336,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -384,35 +384,35 @@
       <c r="O2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>24</v>
@@ -421,13 +421,13 @@
         <v>25</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>24</v>
@@ -477,32 +477,32 @@
       <c r="O3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>42307</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" s="3" t="n">
-        <v>42307</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Y3" s="0" t="s">
         <v>44</v>
@@ -551,8 +551,8 @@
       <c r="O4" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>41</v>
+      <c r="P4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>45</v>
@@ -571,8 +571,8 @@
       <c r="F5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>41</v>
+      <c r="P5" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add handling of transcript files to BatchIngest
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/batch_manifest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t xml:space="preserve">Frances Dickens</t>
   </si>
@@ -94,6 +94,15 @@
     <t xml:space="preserve">Caption Language</t>
   </si>
   <si>
+    <t xml:space="preserve">Transcript File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transcript Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Generated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Skip Transcoding</t>
   </si>
   <si>
@@ -154,10 +163,13 @@
     <t xml:space="preserve">Sheephead Captions</t>
   </si>
   <si>
+    <t xml:space="preserve">Sheephead Transcript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unde aliquid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">file:///tmp/sheephead_mountain_master.mov</t>
@@ -204,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -234,6 +246,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,6 +309,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,17 +338,17 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="12.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -405,179 +427,197 @@
       <c r="V2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AH2" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="S3" s="3" t="n">
         <v>42307</v>
       </c>
       <c r="T3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="AA3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB3" s="4" t="n">
+      <c r="AB3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" s="5" t="n">
         <v>42308</v>
       </c>
-      <c r="AC3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="AF3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" s="5" t="n">
+        <v>42302</v>
+      </c>
+      <c r="AI4" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB4" s="4" t="n">
-        <v>42302</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AA3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
+    <hyperlink ref="AD3" r:id="rId1" display="file:///tmp/sheephead_mountain_master.mov"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>